<commit_message>
[Shubham] Adding update code
</commit_message>
<xml_diff>
--- a/data/excel/dnataHotel.xlsx
+++ b/data/excel/dnataHotel.xlsx
@@ -9,11 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="26" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="27" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="28" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="29" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1716" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2153" uniqueCount="188">
   <si>
     <t>URL</t>
   </si>
@@ -529,13 +531,82 @@
   </si>
   <si>
     <t>dx</t>
+  </si>
+  <si>
+    <t>Shekhar</t>
+  </si>
+  <si>
+    <t>Shekhar@123</t>
+  </si>
+  <si>
+    <t>14-Dec-2023</t>
+  </si>
+  <si>
+    <t>17-Dec-2023</t>
+  </si>
+  <si>
+    <t>//aceuat.dnata.com/backoffice/loginggn.aspx</t>
+  </si>
+  <si>
+    <t>MultiplePassengers</t>
+  </si>
+  <si>
+    <t>AdultName</t>
+  </si>
+  <si>
+    <t>ChildTitle</t>
+  </si>
+  <si>
+    <t>ChildName</t>
+  </si>
+  <si>
+    <t>ChildDOBdate</t>
+  </si>
+  <si>
+    <t>ChildGender</t>
+  </si>
+  <si>
+    <t>Thrilok,RAGHAV,shekhar</t>
+  </si>
+  <si>
+    <t>Devi Shukla,Abhisha Kanal,Abhi Khali</t>
+  </si>
+  <si>
+    <t>Female,Male,Male</t>
+  </si>
+  <si>
+    <t>17-Aug-2023</t>
+  </si>
+  <si>
+    <t>Miss,Master,Master</t>
+  </si>
+  <si>
+    <t>15-Aug-2023</t>
+  </si>
+  <si>
+    <t>5,6,6</t>
+  </si>
+  <si>
+    <t>5,5,6</t>
+  </si>
+  <si>
+    <t>ChildAgeMul</t>
+  </si>
+  <si>
+    <t>20-Jun-2018,25-Jun-2018,13-Jul-2017</t>
+  </si>
+  <si>
+    <t>10-Aug-2023</t>
+  </si>
+  <si>
+    <t>12-Aug-2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -569,8 +640,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -592,6 +670,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -624,7 +708,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -640,6 +724,8 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -958,7 +1044,7 @@
   <dimension ref="A1:AO43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD4"/>
+      <selection activeCell="A2" sqref="A2:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,16 +1231,16 @@
         <v>66</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>67</v>
+        <v>169</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="9">
-        <v>91269126</v>
+      <c r="G2" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>68</v>
+        <v>166</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>69</v>
@@ -1172,10 +1258,10 @@
         <v>76</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>93</v>
+        <v>167</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>94</v>
+        <v>168</v>
       </c>
       <c r="P2" s="1">
         <v>1</v>
@@ -1270,16 +1356,16 @@
         <v>66</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>67</v>
+        <v>169</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G3" s="9">
-        <v>91269126</v>
+      <c r="G3" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>68</v>
+        <v>166</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>69</v>
@@ -1297,10 +1383,10 @@
         <v>76</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>93</v>
+        <v>167</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>94</v>
+        <v>168</v>
       </c>
       <c r="P3" s="1">
         <v>1</v>
@@ -1395,16 +1481,16 @@
         <v>66</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>67</v>
+        <v>169</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G4" s="9">
-        <v>91269126</v>
+      <c r="G4" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>68</v>
+        <v>166</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>69</v>
@@ -1422,10 +1508,10 @@
         <v>76</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>93</v>
+        <v>167</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>94</v>
+        <v>168</v>
       </c>
       <c r="P4" s="1">
         <v>1</v>
@@ -1520,16 +1606,16 @@
         <v>66</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>67</v>
+        <v>169</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G5" s="9">
-        <v>91269126</v>
+      <c r="G5" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>68</v>
+        <v>166</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>69</v>
@@ -1547,10 +1633,10 @@
         <v>76</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>93</v>
+        <v>167</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>94</v>
+        <v>168</v>
       </c>
       <c r="P5" s="1">
         <v>2</v>
@@ -1645,16 +1731,16 @@
         <v>66</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>67</v>
+        <v>169</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G6" s="9">
-        <v>91269126</v>
+      <c r="G6" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>68</v>
+        <v>166</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>69</v>
@@ -1672,10 +1758,10 @@
         <v>76</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>93</v>
+        <v>167</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>94</v>
+        <v>168</v>
       </c>
       <c r="P6" s="1">
         <v>2</v>
@@ -1770,16 +1856,16 @@
         <v>66</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>67</v>
+        <v>169</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G7" s="9">
-        <v>91269126</v>
+      <c r="G7" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>68</v>
+        <v>166</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>69</v>
@@ -1797,10 +1883,10 @@
         <v>76</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>93</v>
+        <v>167</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>94</v>
+        <v>168</v>
       </c>
       <c r="P7" s="1">
         <v>2</v>
@@ -1922,10 +2008,10 @@
         <v>76</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>93</v>
+        <v>167</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>94</v>
+        <v>168</v>
       </c>
       <c r="P8" s="1">
         <v>1</v>
@@ -2047,10 +2133,10 @@
         <v>76</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>93</v>
+        <v>167</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>94</v>
+        <v>168</v>
       </c>
       <c r="P9" s="1">
         <v>1</v>
@@ -2172,10 +2258,10 @@
         <v>76</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>93</v>
+        <v>167</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>94</v>
+        <v>168</v>
       </c>
       <c r="P10" s="1">
         <v>1</v>
@@ -2297,10 +2383,10 @@
         <v>76</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>93</v>
+        <v>167</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>94</v>
+        <v>168</v>
       </c>
       <c r="P11" s="1">
         <v>1</v>
@@ -6383,20 +6469,20 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <dataValidations count="12">
+  <dataValidations count="14">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD15:AD17 AD20:AD22 AD10:AD12 P2:P42">
       <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI2:AI43">
       <formula1>"1 Star,2 Star,3 Star,4 Star,5 Star"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H43">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H43">
       <formula1>"Shekhar123@,Shubham@321"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G43">
       <formula1>"Shekhar,91269126"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E43">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E8:E43">
       <formula1>"//xchange-erp/backoffice/,//dnatauat.quadlabs.net/backoffice/loginggn.aspx"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T43">
@@ -6420,92 +6506,98 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2:AL43">
       <formula1>"Add to Cart,Book"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7">
+      <formula1>"//xchange-erp/backoffice/,//dnatauat.quadlabs.net/backoffice/loginggn.aspx,//aceuat.dnata.com/backoffice/loginggn.aspx"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H7">
+      <formula1>"Tiger@1234,Shubham@321,Shekhar@123"</formula1>
+    </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H2" r:id="rId2" display="Shekhar123@"/>
-    <hyperlink ref="G3" r:id="rId3" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H3" r:id="rId4" display="Shekhar123@"/>
-    <hyperlink ref="G4" r:id="rId5" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H4" r:id="rId6" display="Shekhar123@"/>
-    <hyperlink ref="G5" r:id="rId7" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H5" r:id="rId8" display="Shekhar123@"/>
-    <hyperlink ref="G6" r:id="rId9" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H6" r:id="rId10" display="Shekhar123@"/>
-    <hyperlink ref="G7" r:id="rId11" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H7" r:id="rId12" display="Shekhar123@"/>
-    <hyperlink ref="G8" r:id="rId13" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H8" r:id="rId14" display="Shekhar123@"/>
-    <hyperlink ref="G9" r:id="rId15" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H9" r:id="rId16" display="Shekhar123@"/>
-    <hyperlink ref="G10" r:id="rId17" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H10" r:id="rId18" display="Shekhar123@"/>
-    <hyperlink ref="G11" r:id="rId19" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H11" r:id="rId20" display="Shekhar123@"/>
-    <hyperlink ref="G13" r:id="rId21" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H13" r:id="rId22" display="Shekhar123@"/>
-    <hyperlink ref="G14" r:id="rId23" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H14" r:id="rId24" display="Shekhar123@"/>
-    <hyperlink ref="G15" r:id="rId25" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H15" r:id="rId26" display="Shekhar123@"/>
-    <hyperlink ref="G16" r:id="rId27" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H16" r:id="rId28" display="Shekhar123@"/>
-    <hyperlink ref="G17" r:id="rId29" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H17" r:id="rId30" display="Shekhar123@"/>
-    <hyperlink ref="G18" r:id="rId31" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H18" r:id="rId32" display="Shekhar123@"/>
-    <hyperlink ref="G19" r:id="rId33" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H19" r:id="rId34" display="Shekhar123@"/>
-    <hyperlink ref="G20" r:id="rId35" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H20" r:id="rId36" display="Shekhar123@"/>
-    <hyperlink ref="G21" r:id="rId37" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H21" r:id="rId38" display="Shekhar123@"/>
-    <hyperlink ref="G22" r:id="rId39" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H22" r:id="rId40" display="Shekhar123@"/>
-    <hyperlink ref="G23" r:id="rId41" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H23" r:id="rId42" display="Shekhar123@"/>
-    <hyperlink ref="G24" r:id="rId43" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H24" r:id="rId44" display="Shekhar123@"/>
-    <hyperlink ref="G25" r:id="rId45" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H25" r:id="rId46" display="Shekhar123@"/>
-    <hyperlink ref="G26" r:id="rId47" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H26" r:id="rId48" display="Shekhar123@"/>
-    <hyperlink ref="G27" r:id="rId49" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H27" r:id="rId50" display="Shekhar123@"/>
-    <hyperlink ref="G28" r:id="rId51" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H28" r:id="rId52" display="Shekhar123@"/>
-    <hyperlink ref="G29" r:id="rId53" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H29" r:id="rId54" display="Shekhar123@"/>
-    <hyperlink ref="G30" r:id="rId55" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H30" r:id="rId56" display="Shekhar123@"/>
-    <hyperlink ref="G31" r:id="rId57" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H31" r:id="rId58" display="Shekhar123@"/>
-    <hyperlink ref="G32" r:id="rId59" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H32" r:id="rId60" display="Shekhar123@"/>
-    <hyperlink ref="G33" r:id="rId61" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H33" r:id="rId62" display="Shekhar123@"/>
-    <hyperlink ref="G34" r:id="rId63" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H34" r:id="rId64" display="Shekhar123@"/>
-    <hyperlink ref="G35" r:id="rId65" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H35" r:id="rId66" display="Shekhar123@"/>
-    <hyperlink ref="G36" r:id="rId67" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H36" r:id="rId68" display="Shekhar123@"/>
-    <hyperlink ref="G37" r:id="rId69" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H37" r:id="rId70" display="Shekhar123@"/>
-    <hyperlink ref="G12" r:id="rId71" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H12" r:id="rId72" display="Shekhar123@"/>
-    <hyperlink ref="G38" r:id="rId73" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H38" r:id="rId74" display="Shekhar123@"/>
-    <hyperlink ref="G39" r:id="rId75" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H39" r:id="rId76" display="Shekhar123@"/>
-    <hyperlink ref="G40" r:id="rId77" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H40" r:id="rId78" display="Shekhar123@"/>
-    <hyperlink ref="G41" r:id="rId79" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H41" r:id="rId80" display="Shekhar123@"/>
-    <hyperlink ref="G42" r:id="rId81" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H42" r:id="rId82" display="Shekhar123@"/>
-    <hyperlink ref="G43" r:id="rId83" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H43" r:id="rId84" display="Shekhar123@"/>
+    <hyperlink ref="G8" r:id="rId1" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H8" r:id="rId2" display="Shekhar123@"/>
+    <hyperlink ref="G9" r:id="rId3" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H9" r:id="rId4" display="Shekhar123@"/>
+    <hyperlink ref="G10" r:id="rId5" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H10" r:id="rId6" display="Shekhar123@"/>
+    <hyperlink ref="G11" r:id="rId7" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H11" r:id="rId8" display="Shekhar123@"/>
+    <hyperlink ref="G13" r:id="rId9" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H13" r:id="rId10" display="Shekhar123@"/>
+    <hyperlink ref="G14" r:id="rId11" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H14" r:id="rId12" display="Shekhar123@"/>
+    <hyperlink ref="G15" r:id="rId13" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H15" r:id="rId14" display="Shekhar123@"/>
+    <hyperlink ref="G16" r:id="rId15" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H16" r:id="rId16" display="Shekhar123@"/>
+    <hyperlink ref="G17" r:id="rId17" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H17" r:id="rId18" display="Shekhar123@"/>
+    <hyperlink ref="G18" r:id="rId19" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H18" r:id="rId20" display="Shekhar123@"/>
+    <hyperlink ref="G19" r:id="rId21" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H19" r:id="rId22" display="Shekhar123@"/>
+    <hyperlink ref="G20" r:id="rId23" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H20" r:id="rId24" display="Shekhar123@"/>
+    <hyperlink ref="G21" r:id="rId25" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H21" r:id="rId26" display="Shekhar123@"/>
+    <hyperlink ref="G22" r:id="rId27" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H22" r:id="rId28" display="Shekhar123@"/>
+    <hyperlink ref="G23" r:id="rId29" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H23" r:id="rId30" display="Shekhar123@"/>
+    <hyperlink ref="G24" r:id="rId31" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H24" r:id="rId32" display="Shekhar123@"/>
+    <hyperlink ref="G25" r:id="rId33" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H25" r:id="rId34" display="Shekhar123@"/>
+    <hyperlink ref="G26" r:id="rId35" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H26" r:id="rId36" display="Shekhar123@"/>
+    <hyperlink ref="G27" r:id="rId37" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H27" r:id="rId38" display="Shekhar123@"/>
+    <hyperlink ref="G28" r:id="rId39" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H28" r:id="rId40" display="Shekhar123@"/>
+    <hyperlink ref="G29" r:id="rId41" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H29" r:id="rId42" display="Shekhar123@"/>
+    <hyperlink ref="G30" r:id="rId43" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H30" r:id="rId44" display="Shekhar123@"/>
+    <hyperlink ref="G31" r:id="rId45" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H31" r:id="rId46" display="Shekhar123@"/>
+    <hyperlink ref="G32" r:id="rId47" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H32" r:id="rId48" display="Shekhar123@"/>
+    <hyperlink ref="G33" r:id="rId49" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H33" r:id="rId50" display="Shekhar123@"/>
+    <hyperlink ref="G34" r:id="rId51" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H34" r:id="rId52" display="Shekhar123@"/>
+    <hyperlink ref="G35" r:id="rId53" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H35" r:id="rId54" display="Shekhar123@"/>
+    <hyperlink ref="G36" r:id="rId55" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H36" r:id="rId56" display="Shekhar123@"/>
+    <hyperlink ref="G37" r:id="rId57" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H37" r:id="rId58" display="Shekhar123@"/>
+    <hyperlink ref="G12" r:id="rId59" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H12" r:id="rId60" display="Shekhar123@"/>
+    <hyperlink ref="G38" r:id="rId61" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H38" r:id="rId62" display="Shekhar123@"/>
+    <hyperlink ref="G39" r:id="rId63" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H39" r:id="rId64" display="Shekhar123@"/>
+    <hyperlink ref="G40" r:id="rId65" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H40" r:id="rId66" display="Shekhar123@"/>
+    <hyperlink ref="G41" r:id="rId67" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H41" r:id="rId68" display="Shekhar123@"/>
+    <hyperlink ref="G42" r:id="rId69" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H42" r:id="rId70" display="Shekhar123@"/>
+    <hyperlink ref="G43" r:id="rId71" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H43" r:id="rId72" display="Shekhar123@"/>
+    <hyperlink ref="H2" r:id="rId73" display="Shekhar123@"/>
+    <hyperlink ref="G2" r:id="rId74" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H3" r:id="rId75" display="Shekhar123@"/>
+    <hyperlink ref="G3" r:id="rId76" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H4" r:id="rId77" display="Shekhar123@"/>
+    <hyperlink ref="G4" r:id="rId78" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H5" r:id="rId79" display="Shekhar123@"/>
+    <hyperlink ref="G5" r:id="rId80" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H6" r:id="rId81" display="Shekhar123@"/>
+    <hyperlink ref="G6" r:id="rId82" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H7" r:id="rId83" display="Shekhar123@"/>
+    <hyperlink ref="G7" r:id="rId84" display="shubham.natkar@quadlabs.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId85"/>
@@ -6514,10 +6606,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO2"/>
+  <dimension ref="A1:AO6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8:K9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6692,28 +6784,28 @@
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>66</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>67</v>
+        <v>169</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="9">
-        <v>91269126</v>
+      <c r="G2" s="9" t="s">
+        <v>165</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>68</v>
+        <v>166</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>69</v>
@@ -6731,10 +6823,10 @@
         <v>76</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>93</v>
+        <v>167</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>94</v>
+        <v>168</v>
       </c>
       <c r="P2" s="1">
         <v>1</v>
@@ -6812,16 +6904,1595 @@
         <v>86</v>
       </c>
       <c r="AO2" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="P3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO3" s="1" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="P4" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI4" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AM4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO4" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="P5" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AB5" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD5" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AK5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL5" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO5" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="P6" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AB6" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI6" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AK6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO6" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2:AL6">
+      <formula1>"Add to Cart,Book"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO2:AO6">
+      <formula1>"Quote,Fulfilment"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ2:AJ6 AH2:AH6 V2:W6 AC2:AC6 Z2:Z6">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B6">
+      <formula1>"Positive,Negative"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J6">
+      <formula1>"BusinessTravel,Personal"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K6">
+      <formula1>"Individual,Dependent,MultiplePassengers,GuestUser"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T6">
+      <formula1>"FOP - Credit Card,FOP - Corporate Card,FOP - Credit Limit,FOP - Deposit Voucher,FOP - Gift Voucher,FOP - Debit Card,FOP - Cash"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G6">
+      <formula1>"Shekhar,91269126"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI2:AI6">
+      <formula1>"1 Star,2 Star,3 Star,4 Star,5 Star"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P6">
+      <formula1>"1,2,3,4,5"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H6">
+      <formula1>"Tiger@1234,Shubham@321,Shekhar@123"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6">
+      <formula1>"//xchange-erp/backoffice/,//dnatauat.quadlabs.net/backoffice/loginggn.aspx,//aceuat.dnata.com/backoffice/loginggn.aspx"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" display="Shekhar123@"/>
+    <hyperlink ref="G2" r:id="rId2" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H3" r:id="rId3" display="Shekhar123@"/>
+    <hyperlink ref="G3" r:id="rId4" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H4" r:id="rId5" display="Shekhar123@"/>
+    <hyperlink ref="G4" r:id="rId6" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H5" r:id="rId7" display="Shekhar123@"/>
+    <hyperlink ref="G5" r:id="rId8" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H6" r:id="rId9" display="Shekhar123@"/>
+    <hyperlink ref="G6" r:id="rId10" display="shubham.natkar@quadlabs.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AU4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="AN28" sqref="AN28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL1" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="AM1" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN1" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO1" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="AP1" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="AQ1" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="AR1" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="AS1" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="AT1" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="AU1" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="P2" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AP2" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="AQ2" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="AR2" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="AS2" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="AT2" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="P3" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO3" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AP3" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="AQ3" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="AR3" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="AS3" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="AT3" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="AU3" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="P4" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI4" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AM4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO4" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AP4" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="AQ4" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="AR4" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="AS4" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="AT4" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="AU4" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU2:AU4">
+      <formula1>"Quote,Fulfilment"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E4">
+      <formula1>"//xchange-erp/backoffice/,//dnatauat.quadlabs.net/backoffice/loginggn.aspx,//aceuat.dnata.com/backoffice/loginggn.aspx"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H4">
+      <formula1>"Tiger@1234,Shubham@321,Shekhar@123"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P4">
+      <formula1>"1,2,3,4,5"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI2:AI4">
+      <formula1>"1 Star,2 Star,3 Star,4 Star,5 Star"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G4">
+      <formula1>"Shekhar,91269126"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T4">
+      <formula1>"FOP - Credit Card,FOP - Corporate Card,FOP - Credit Limit,FOP - Deposit Voucher,FOP - Gift Voucher,FOP - Debit Card,FOP - Cash"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K4">
+      <formula1>"Individual,Dependent,MultiplePassengers,GuestUser"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4">
+      <formula1>"BusinessTravel,Personal"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B4">
+      <formula1>"Positive,Negative"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ2:AJ4 AH2:AH4 V2:W4 AC2:AC4 Z2:Z4">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2:AL4">
+      <formula1>"Add to Cart,Book"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" display="Shekhar123@"/>
+    <hyperlink ref="G2" r:id="rId2" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H3" r:id="rId3" display="Shekhar123@"/>
+    <hyperlink ref="G3" r:id="rId4" display="shubham.natkar@quadlabs.com"/>
+    <hyperlink ref="H4" r:id="rId5" display="Shekhar123@"/>
+    <hyperlink ref="G4" r:id="rId6" display="shubham.natkar@quadlabs.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AU2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="AL1" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="AM1" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="AN1" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="AO1" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="AP1" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="AQ1" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="AR1" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="AS1" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="AT1" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="AU1" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="P2" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO2" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AP2" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="AQ2" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="AR2" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="AS2" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="AT2" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="AU2" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="12">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2">
       <formula1>"Add to Cart,Book"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO2">
-      <formula1>"Quote,Fulfilment"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ2 AH2 V2:W2 AC2 Z2">
       <formula1>"Yes,No"</formula1>
@@ -6838,14 +8509,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2">
       <formula1>"FOP - Credit Card,FOP - Corporate Card,FOP - Credit Limit,FOP - Deposit Voucher,FOP - Gift Voucher,FOP - Debit Card,FOP - Cash"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2">
-      <formula1>"//xchange-erp/backoffice/,//dnatauat.quadlabs.net/backoffice/loginggn.aspx"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
       <formula1>"Shekhar,91269126"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2">
-      <formula1>"Shekhar123@,Shubham@321"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI2">
       <formula1>"1 Star,2 Star,3 Star,4 Star,5 Star"</formula1>
@@ -6853,10 +8518,19 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2">
       <formula1>"1,2,3,4,5"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2">
+      <formula1>"Tiger@1234,Shubham@321,Shekhar@123"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2">
+      <formula1>"//xchange-erp/backoffice/,//dnatauat.quadlabs.net/backoffice/loginggn.aspx,//aceuat.dnata.com/backoffice/loginggn.aspx"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU2">
+      <formula1>"Quote,Fulfilment"</formula1>
+    </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" display="shubham.natkar@quadlabs.com"/>
-    <hyperlink ref="H2" r:id="rId2" display="Shekhar123@"/>
+    <hyperlink ref="H2" r:id="rId1" display="Shekhar123@"/>
+    <hyperlink ref="G2" r:id="rId2" display="shubham.natkar@quadlabs.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>